<commit_message>
--them co so y tế và sửa thành công chức năng lập phiếu
</commit_message>
<xml_diff>
--- a/storage/app/public/data/CoSoYTe/CoSoYTe.xlsx
+++ b/storage/app/public/data/CoSoYTe/CoSoYTe.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B38106-B976-4773-943C-85ECB07D0650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Sở y tế An Giang</t>
   </si>
@@ -47,12 +46,45 @@
   </si>
   <si>
     <t>Tên cơ sở y tế</t>
+  </si>
+  <si>
+    <t>Trạm y tế Phường Mỹ Bình</t>
+  </si>
+  <si>
+    <t>Trạm y tế Phường Mỹ Xuyên</t>
+  </si>
+  <si>
+    <t>Trạm y tế Phường Đông Xuyên</t>
+  </si>
+  <si>
+    <t>Trạm y tế Phường Mỹ Phước</t>
+  </si>
+  <si>
+    <t>Trạm y tế Phường Mỹ Quý</t>
+  </si>
+  <si>
+    <t>Trạm y tế Phường Mỹ Thới</t>
+  </si>
+  <si>
+    <t>Trạm y tế Phường Mỹ Thạnh</t>
+  </si>
+  <si>
+    <t>Trạm y tế Phường Bình Khánh</t>
+  </si>
+  <si>
+    <t>Trạm y tế Phường Bình Đức</t>
+  </si>
+  <si>
+    <t>Trạm y tế Xã Mỹ Khánh</t>
+  </si>
+  <si>
+    <t>Trạm y tế Xã Mỹ Hòa Hưng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -363,22 +395,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -395,7 +427,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -406,7 +438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -420,7 +452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -431,13 +463,13 @@
         <v>78</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -448,10 +480,194 @@
         <v>78</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>2</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>78</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>78</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>78</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>78</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>78</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>78</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>78</v>
+      </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>78</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>78</v>
+      </c>
+      <c r="D14">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>78</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>78</v>
+      </c>
+      <c r="D16">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
giao diện phieu xuất và xử lý xác nhận phiếu nhập bên trung tâm y tê
</commit_message>
<xml_diff>
--- a/storage/app/public/data/CoSoYTe/CoSoYTe.xlsx
+++ b/storage/app/public/data/CoSoYTe/CoSoYTe.xlsx
@@ -399,7 +399,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,6 +657,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
       <c r="B16">
         <v>5</v>
       </c>

</xml_diff>